<commit_message>
Updated the indicator list to include releases from Norway, Sweden, Poland, Russia, Turkey & ECB. Then Scraped the news data for those events and downloaded USDNOK tick data for Norway's GDP
</commit_message>
<xml_diff>
--- a/haawks-indicator-shortlist.xlsx
+++ b/haawks-indicator-shortlist.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="567">
   <si>
     <t xml:space="preserve">Indicator</t>
   </si>
@@ -1491,14 +1491,321 @@
   <si>
     <t xml:space="preserve">Gross Domestic Product (GDP) measures the annualized change in the inflation-adjusted value of all goods and services produced by the economy. It is the broadest measure of economic activity and the primary indicator of the economy''s health. A stronger than expected number should be taken as positive for the CAD and a lower than expected number as negative to the CAD.</t>
   </si>
+  <si>
+    <t xml:space="preserve">Norway GDP QoQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SSB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00091;0.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norway Gross Domestic Product (GDP) QoQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Statistisk Sentralbyra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gross Domestic Product (GDP) measures the annualized change in the inflation-adjusted value of all goods and services produced by the economy. It is the broadest measure of economic activity and the primary indicator of the economy's health.
+A higher than expected reading should be taken as positive/bullish for the NOK, while a lower than expected reading should be taken as negative/bearish for the NOK.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norway GDP Mainland QoQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00092;0.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norway Gross Domestic Product (GDP) Mainland QoQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Statistics Norway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GDP measures summary value of goods and services generated in a relevant country or region. A region's gross domestic product, or GDP, is one of the ways for measuring the size of its economy. Expenditure approach - Total expenditures on all finished goods and services produced within the economy. Calculation: GDP using the expenditure approach is derived as the sum of all final expenditures, changes in inventories and exports of goods and services less imports of goods and services. Market influence of GDP: Unexpectedly high quarterly GDP growth is perceived to be potentially inflationary if the economy is close to full capacity; this, in turn, causes bond prices to drop and yields and interest rates to rise. Where the stock market is concerned on one side higher than expected growth leads to higher profits and that's good for the stock market. On the other, it may increase expected inflation and lead to higher interest rates that are bad for the stock market.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norway Core Retail Sales MoM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00047;0.1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retail sales data represents total consumer purchase from retail stores. It provides valuable information about consumer spending which makes up the consumption part of GDP.
+A higher than expected reading should be taken as positive/bullish for the NOK , while a lower than expected reading should be taken as negative/bearish for the NOK.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norway Unemployment Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00049;3.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LFS- Labour Force Survey. Three-months moving average. Employed persons are persons aged 16-74 who performed work for pay or profit for at least one hour in the survey week, or who were temporarily absent from work because of illness,holidays etc. Conscripts are classified as employed persons. Persons engaged by government measures to promote employment are also included if they receive wages. Unemployed persons are persons who were not employed in the survey week,but who had been seeking work during the preceding four weeks, and were available for work within the next two weeks. Persons in the labour force are either employed or unemployed. The remaining group of persons is labelled not in the labour force. Unemployed persons and persons not in the labour force constitute the group non-employed persons.
+A higher than expected reading should be taken as negative/bearish for the NOK , while a lower than expected reading should be taken as positive/bullish for the NOK.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norway CPI MoM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00041;1.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norway Consumer Price Index (CPI) MoM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The consumer price index (CPI) is a measure of change over a specified period of time in the general level of prices of goods and services that a given population acquires, uses or pays for consumption. It compares a household's cost for a specific basket of finished goods and services with the cost of the same basket during an earlier benchmark period.
+A higher than expected reading should be taken as positive/bullish for the NOK , while a lower than expected reading should be taken as negative/bearish for the NOK.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norway CPI YoY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00042;6.9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norway Consumer Price Index (CPI) YoY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norges Bank Interest Rate Decision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00017;1.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norway Interest Rate Decision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norges Bank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Norges Bank Monetary Policy Committee's decision on where to set the overnight deposit rate. Traders watch interest rate changes closely as short term interest rates are the primary factor in currency valuation.
+A higher than expected rate is positive/bullish for the NOK, while a lower than expected rate is negative/bearish for the NOK.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden GDP QoQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00071;0.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden Gross Domestic Product (GDP) QoQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Statistiska Centralbyran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gross Domestic Product (GDP) measures the annualized change in the inflation-adjusted value of all goods and services produced by the economy. It is the broadest measure of economic activity and the primary indicator of the economy's health. The quarterly change measures the seasonally adjusted change in percentage compared to the previous quarter. A higher than expected reading should be taken as positive/bullish for the SEK, while a lower than expected reading should be taken as negative/bearish for the SEK.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden GDP YoY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00072;2.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden Gross Domestic Product (GDP) YoY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gross Domestic Product (GDP) measures the annualized change in the inflation-adjusted value of all goods and services produced by the economy. It is the broadest measure of economic activity and the primary indicator of the economy's health. The year-on-year change measures the seasonally adjusted change in percentage during a quarter compared to the equivalent period during the previous year. A higher than expected reading should be taken as positive/bullish for the SEK, while a lower than expected reading should be taken as negative/bearish for the SEK.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden Retail Sales MoM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00057;-0.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCB - Statistics Sweden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retail trade excluding motor vehicles; including repair shops for personal and household goods.Adjusted for irregularity of the calendar.Retail sales data represents total consumer purchase from retail stores. It provides valuable information about consumer spending which makes up the consumption part of GDP.
+A higher than expected reading should be taken as positive/bullish for the SEK , while a lower than expected reading should be taken as negative/bearish for the SEK.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden Retail Sales YoY</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 00058;-5.1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden Unemployment Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00059;6.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The definition for an unemployed person is: Persons (16-65 years) who were available for work (except for temporary illness) but did not work during the survey week, and who made specific efforts to find a job within the previous 4 weeks by going to an employment agency, by applying directly to an employer, by answering a job ad, or being on a union or professional register. The percentage number is calculated unemployed / (employed + unemployed).
+A higher than expected reading should be taken as negative/bearish for the SEK , while a lower than expected reading should be taken as positive/bullish for the SEK.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden CPI MoM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00051;1.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden Consumer Price Index (CPI) MoM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Consumer Price Index (CPI) measures the change in the price of goods and services from the perspective of the consumer. It is a key way to measure changes in purchasing trends and inflation.
+A higher than expected reading should be taken as positive/bullish for the SEK, while a lower than expected reading should be taken as negative/bearish for the SEK.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden CPI YoY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00052;10.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden Consumer Price Index (CPI) YoY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden CPIF MoM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00053;1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden Consumer Price Index at Constant Interest Rates (CPIF) MoM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden, Consumer Prices, By Commodity, Special Indexes, Underlying inflation CPIF, Index. The Underlying Inflation Rate according to CPIF (CPI at constant interest rates) differs from CPI by keeping interest rate for households mortgage interest payment at a constant rate. CPIF is calculated on request fromSveriges Riksbank (the Swedish central bank).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden CPIF YoY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00054;9.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden Consumer Price Index at Constant Interest Rates (CPIF) YoY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poland Interest Rate Decision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NBP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00141;6.75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Narodowy Bank Polski</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The National Bank of Poland (NBP) Monetary Policy Committee's decision on where to set the benchmark interest rate. Traders watch interest rate changes closely as short term interest rates are the primary factor in currency valuation.
+A higher than expected rate is positive/bullish for the PLN, while a lower than expected rate is negative/bearish for the PLN.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank of Russia Interest Rate Decision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Russia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CBR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00003;7.50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Russia Interest Rate Decision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RUB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central Bank of Russia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Bank Rossii decision on short term interest rate. The decision on where to set interest rates depends mostly on growth outlook and inflation. The primary objective of the central bank is to achieve price stability. High interest rates attract foreigners looking for the best "risk-free" return on their money, which can dramatically increases demand for the nation's currency.
+A higher than expected rate is positive/bullish for the RUB, while a lower than expected rate is negative/bearish for the RUB.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECB Main Refinancing Operations Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">European Union</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00021;1.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eurozone Interest Rate Decision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">European Central Bank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The six members of the European Central Bank (ECB) Executive Board and the 16 governors of the euro area central banks vote on where to set the rate. Traders watch interest rate changes closely as short term interest rates are the primary factor in currency valuation.
+A higher than expected rate is positive/bullish for the EUR, while a lower than expected rate is negative/bearish for the EUR.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turkey One-Week Repo Rate (policy rate)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turkey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCMB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00013;10.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Turkey One-Week Repo Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central Bank of the Republic of Turkey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Central Bank of the Republic of Turkey's (CBRT) Monetary Policy Committee votes on where to set the overnight interest rate. Traders watch interest rate changes closely as short term interest rates are the primary factor in currency valuation.
+A higher than expected rate is positive/bullish for the TRY, while a lower than expected rate is negative/bearish for the TRY.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="00000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -1580,7 +1887,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1601,6 +1908,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1618,16 +1929,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y88"/>
+  <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L60" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T66" activeCellId="0" sqref="T66"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Z2" activeCellId="0" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="33.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="28.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="33.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16226" style="1" width="11.53"/>
   </cols>
   <sheetData>
@@ -1773,16 +2084,16 @@
         <v>40</v>
       </c>
       <c r="V2" s="1" t="n">
-        <v>1.139</v>
+        <v>1</v>
       </c>
       <c r="W2" s="1" t="n">
-        <v>2.353</v>
+        <v>2</v>
       </c>
       <c r="X2" s="1" t="n">
-        <v>3.672</v>
+        <v>3</v>
       </c>
       <c r="Y2" s="1" t="n">
-        <v>5.908</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1850,16 +2161,16 @@
         <v>40</v>
       </c>
       <c r="V3" s="1" t="n">
-        <v>0.584</v>
+        <v>0.5</v>
       </c>
       <c r="W3" s="1" t="n">
-        <v>1.284</v>
+        <v>1</v>
       </c>
       <c r="X3" s="1" t="n">
-        <v>2.173</v>
+        <v>2</v>
       </c>
       <c r="Y3" s="1" t="n">
-        <v>3.271</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1992,16 +2303,16 @@
         <v>40</v>
       </c>
       <c r="V5" s="1" t="n">
-        <v>0.187</v>
+        <v>0.2</v>
       </c>
       <c r="W5" s="1" t="n">
-        <v>0.395</v>
+        <v>0.4</v>
       </c>
       <c r="X5" s="1" t="n">
-        <v>0.621</v>
+        <v>0.6</v>
       </c>
       <c r="Y5" s="1" t="n">
-        <v>1.017</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8251,6 +8562,1291 @@
         <v>2.3</v>
       </c>
     </row>
+    <row r="89" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="J89" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="K89" s="1" t="n">
+        <v>44008</v>
+      </c>
+      <c r="M89" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="N89" s="1" t="n">
+        <v>443</v>
+      </c>
+      <c r="O89" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="P89" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q89" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="R89" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="S89" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="T89" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U89" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V89" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="W89" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="X89" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Y89" s="1" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="J90" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="K90" s="1" t="n">
+        <v>44008</v>
+      </c>
+      <c r="M90" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="N90" s="1" t="n">
+        <v>1257</v>
+      </c>
+      <c r="O90" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="P90" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q90" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="R90" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="S90" s="1" t="s">
+        <v>481</v>
+      </c>
+      <c r="T90" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U90" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V90" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="W90" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="X90" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="Y90" s="1" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="J91" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="K91" s="1" t="n">
+        <v>44008</v>
+      </c>
+      <c r="M91" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="N91" s="1" t="n">
+        <v>640</v>
+      </c>
+      <c r="O91" s="1" t="s">
+        <v>482</v>
+      </c>
+      <c r="P91" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q91" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="R91" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="S91" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="T91" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U91" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V91" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="W91" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="X91" s="1" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="Y91" s="1" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="J92" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="K92" s="1" t="n">
+        <v>44008</v>
+      </c>
+      <c r="M92" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="N92" s="1" t="n">
+        <v>638</v>
+      </c>
+      <c r="O92" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="P92" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q92" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="R92" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="S92" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="T92" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U92" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="V92" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="W92" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="X92" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="Y92" s="1" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="J93" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="K93" s="1" t="n">
+        <v>44008</v>
+      </c>
+      <c r="M93" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="N93" s="1" t="n">
+        <v>637</v>
+      </c>
+      <c r="O93" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="P93" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q93" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="R93" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="S93" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="T93" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U93" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V93" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="W93" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="X93" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="Y93" s="1" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="J94" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="K94" s="1" t="n">
+        <v>44008</v>
+      </c>
+      <c r="M94" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="N94" s="1" t="n">
+        <v>1179</v>
+      </c>
+      <c r="O94" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="P94" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q94" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="R94" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="S94" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="T94" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U94" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V94" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="W94" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="X94" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="Y94" s="1" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="J95" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="K95" s="1" t="n">
+        <v>44008</v>
+      </c>
+      <c r="M95" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="N95" s="1" t="n">
+        <v>444</v>
+      </c>
+      <c r="O95" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="P95" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q95" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="R95" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="S95" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="T95" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U95" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V95" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W95" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X95" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y95" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="J96" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="K96" s="1" t="n">
+        <v>44008</v>
+      </c>
+      <c r="M96" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="N96" s="1" t="n">
+        <v>426</v>
+      </c>
+      <c r="O96" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="P96" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q96" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="R96" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="S96" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="T96" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U96" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V96" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="W96" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="X96" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="Y96" s="1" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="J97" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="K97" s="1" t="n">
+        <v>44008</v>
+      </c>
+      <c r="M97" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="N97" s="1" t="n">
+        <v>1186</v>
+      </c>
+      <c r="O97" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="P97" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q97" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="R97" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="S97" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="T97" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U97" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V97" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="W97" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="X97" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="Y97" s="1" t="n">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="J98" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="K98" s="1" t="n">
+        <v>44008</v>
+      </c>
+      <c r="M98" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="N98" s="1" t="n">
+        <v>626</v>
+      </c>
+      <c r="O98" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="P98" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q98" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="R98" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="S98" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="T98" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U98" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V98" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="W98" s="1" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="X98" s="1" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="Y98" s="1" t="n">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="J99" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="K99" s="1" t="n">
+        <v>44008</v>
+      </c>
+      <c r="M99" s="1" t="s">
+        <v>518</v>
+      </c>
+      <c r="N99" s="1" t="n">
+        <v>1189</v>
+      </c>
+      <c r="O99" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="P99" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q99" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="R99" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="S99" s="3" t="s">
+        <v>516</v>
+      </c>
+      <c r="T99" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U99" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V99" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="W99" s="1" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="X99" s="1" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="Y99" s="1" t="n">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="J100" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="K100" s="1" t="n">
+        <v>44008</v>
+      </c>
+      <c r="M100" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="N100" s="1" t="n">
+        <v>627</v>
+      </c>
+      <c r="O100" s="1" t="s">
+        <v>519</v>
+      </c>
+      <c r="P100" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q100" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="R100" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="S100" s="3" t="s">
+        <v>521</v>
+      </c>
+      <c r="T100" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U100" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="V100" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="W100" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="X100" s="1" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="Y100" s="1" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="J101" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="K101" s="1" t="n">
+        <v>44008</v>
+      </c>
+      <c r="M101" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="N101" s="1" t="n">
+        <v>1185</v>
+      </c>
+      <c r="O101" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="P101" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q101" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="R101" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="S101" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="T101" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U101" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V101" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W101" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="X101" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Y101" s="1" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="J102" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="K102" s="1" t="n">
+        <v>44008</v>
+      </c>
+      <c r="M102" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="N102" s="1" t="n">
+        <v>425</v>
+      </c>
+      <c r="O102" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="P102" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q102" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="R102" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="S102" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="T102" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U102" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V102" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W102" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="X102" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Y102" s="1" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="J103" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="K103" s="1" t="n">
+        <v>44008</v>
+      </c>
+      <c r="M103" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="N103" s="1" t="n">
+        <v>1213</v>
+      </c>
+      <c r="O103" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="P103" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q103" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="R103" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="S103" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="T103" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U103" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V103" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="W103" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="X103" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Y103" s="1" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="J104" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="K104" s="1" t="n">
+        <v>44008</v>
+      </c>
+      <c r="M104" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="N104" s="1" t="n">
+        <v>1214</v>
+      </c>
+      <c r="O104" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="P104" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q104" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="R104" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="S104" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="T104" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U104" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V104" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="W104" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="X104" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="Y104" s="1" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="J105" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="K105" s="1" t="n">
+        <v>44008</v>
+      </c>
+      <c r="M105" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="N105" s="1" t="n">
+        <v>447</v>
+      </c>
+      <c r="O105" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="P105" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q105" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="R105" s="1" t="s">
+        <v>541</v>
+      </c>
+      <c r="S105" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="T105" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U105" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V105" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W105" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X105" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y105" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="1" t="s">
+        <v>543</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="J106" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="K106" s="1" t="n">
+        <v>44008</v>
+      </c>
+      <c r="M106" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="N106" s="1" t="n">
+        <v>554</v>
+      </c>
+      <c r="O106" s="1" t="s">
+        <v>547</v>
+      </c>
+      <c r="P106" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q106" s="1" t="s">
+        <v>548</v>
+      </c>
+      <c r="R106" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="S106" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="T106" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U106" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V106" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W106" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X106" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y106" s="1" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>553</v>
+      </c>
+      <c r="J107" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="K107" s="1" t="n">
+        <v>44008</v>
+      </c>
+      <c r="M107" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="N107" s="1" t="n">
+        <v>164</v>
+      </c>
+      <c r="O107" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="P107" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q107" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="R107" s="1" t="s">
+        <v>557</v>
+      </c>
+      <c r="S107" s="3" t="s">
+        <v>558</v>
+      </c>
+      <c r="T107" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U107" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V107" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W107" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X107" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y107" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>561</v>
+      </c>
+      <c r="J108" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="K108" s="1" t="n">
+        <v>44008</v>
+      </c>
+      <c r="M108" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="N108" s="1" t="n">
+        <v>409</v>
+      </c>
+      <c r="O108" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="P108" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q108" s="1" t="s">
+        <v>564</v>
+      </c>
+      <c r="R108" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="S108" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="T108" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="U108" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V108" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="W108" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="X108" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y108" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J109" s="5"/>
+    </row>
+    <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J110" s="5"/>
+    </row>
+    <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J111" s="5"/>
+    </row>
+    <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J112" s="5"/>
+    </row>
+    <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J113" s="5"/>
+    </row>
+    <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J114" s="5"/>
+    </row>
+    <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J115" s="5"/>
+    </row>
+    <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J116" s="5"/>
+    </row>
+    <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J117" s="5"/>
+    </row>
+    <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J118" s="5"/>
+    </row>
+    <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J119" s="5"/>
+    </row>
+    <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J120" s="5"/>
+    </row>
+    <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J121" s="5"/>
+    </row>
+    <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J122" s="5"/>
+    </row>
+    <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J123" s="5"/>
+    </row>
+    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J124" s="5"/>
+    </row>
+    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J125" s="5"/>
+    </row>
+    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J126" s="5"/>
+    </row>
+    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J127" s="5"/>
+    </row>
+    <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J128" s="5"/>
+    </row>
+    <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J129" s="5"/>
+    </row>
+    <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J130" s="5"/>
+    </row>
+    <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J131" s="5"/>
+    </row>
+    <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J132" s="5"/>
+    </row>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
added functions to turn news pip metrics into dataframes. Next step is to generate pdf reports with these dataframes
</commit_message>
<xml_diff>
--- a/haawks-indicator-shortlist.xlsx
+++ b/haawks-indicator-shortlist.xlsx
@@ -1931,8 +1931,8 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z2" activeCellId="0" sqref="Z2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J92" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Z101" activeCellId="0" sqref="Z101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8798,7 +8798,7 @@
         <v>0.1</v>
       </c>
       <c r="W92" s="1" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="X92" s="1" t="n">
         <v>0.3</v>
@@ -9326,16 +9326,16 @@
         <v>75</v>
       </c>
       <c r="V101" s="1" t="n">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="W101" s="1" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="X101" s="1" t="n">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="Y101" s="1" t="n">
-        <v>0.3</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
modified calc_news_pip_metrics to skip triggers which are 0. Also modified load_news_pip_data to handle corrupted/empty tick data files which happens occasionally when downloading from dukascopy
</commit_message>
<xml_diff>
--- a/haawks-indicator-shortlist.xlsx
+++ b/haawks-indicator-shortlist.xlsx
@@ -1931,8 +1931,8 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J92" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z101" activeCellId="0" sqref="Z101"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Z77" activeCellId="0" sqref="Z77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7739,16 +7739,16 @@
         <v>75</v>
       </c>
       <c r="V77" s="1" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="W77" s="1" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="X77" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="Y77" s="1" t="n">
         <v>0</v>
-      </c>
-      <c r="W77" s="1" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="X77" s="1" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="Y77" s="1" t="n">
-        <v>0.3</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
fixed a couple of bugs that were crashing ranker.py, still running ranker.py
</commit_message>
<xml_diff>
--- a/haawks-indicator-shortlist.xlsx
+++ b/haawks-indicator-shortlist.xlsx
@@ -1769,8 +1769,8 @@
   </sheetPr>
   <dimension ref="A1:Z1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3850,7 +3850,7 @@
       <c r="Y26" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Z26" s="0" t="s">
+      <c r="Z26" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3930,7 +3930,7 @@
       <c r="Y27" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Z27" s="0" t="s">
+      <c r="Z27" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -4010,7 +4010,7 @@
       <c r="Y28" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="Z28" s="0" t="s">
+      <c r="Z28" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -4090,7 +4090,7 @@
       <c r="Y29" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Z29" s="0" t="s">
+      <c r="Z29" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -4170,7 +4170,7 @@
       <c r="Y30" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="Z30" s="0" t="s">
+      <c r="Z30" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -4247,7 +4247,7 @@
       <c r="Y31" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="Z31" s="0" t="s">
+      <c r="Z31" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -4327,7 +4327,7 @@
       <c r="Y32" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Z32" s="0" t="s">
+      <c r="Z32" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -4404,7 +4404,7 @@
       <c r="Y33" s="1" t="n">
         <v>3.5</v>
       </c>
-      <c r="Z33" s="0" t="s">
+      <c r="Z33" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -4484,7 +4484,7 @@
       <c r="Y34" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="Z34" s="0" t="s">
+      <c r="Z34" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -4564,7 +4564,7 @@
       <c r="Y35" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="Z35" s="0" t="s">
+      <c r="Z35" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -4644,7 +4644,7 @@
       <c r="Y36" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="Z36" s="0" t="s">
+      <c r="Z36" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -4724,7 +4724,7 @@
       <c r="Y37" s="1" t="n">
         <v>0.9</v>
       </c>
-      <c r="Z37" s="0" t="s">
+      <c r="Z37" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -4804,7 +4804,7 @@
       <c r="Y38" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="Z38" s="0" t="s">
+      <c r="Z38" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -4884,7 +4884,7 @@
       <c r="Y39" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Z39" s="0" t="s">
+      <c r="Z39" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -4964,7 +4964,7 @@
       <c r="Y40" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="Z40" s="0" t="s">
+      <c r="Z40" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -5044,7 +5044,7 @@
       <c r="Y41" s="1" t="n">
         <v>0.1</v>
       </c>
-      <c r="Z41" s="0" t="s">
+      <c r="Z41" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -5124,7 +5124,7 @@
       <c r="Y42" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="Z42" s="0" t="s">
+      <c r="Z42" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -5204,7 +5204,7 @@
       <c r="Y43" s="1" t="n">
         <v>0.09</v>
       </c>
-      <c r="Z43" s="0" t="s">
+      <c r="Z43" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -5284,7 +5284,7 @@
       <c r="Y44" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="Z44" s="0" t="s">
+      <c r="Z44" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -5364,7 +5364,7 @@
       <c r="Y45" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="Z45" s="0" t="s">
+      <c r="Z45" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -5444,7 +5444,7 @@
       <c r="Y46" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="Z46" s="0" t="s">
+      <c r="Z46" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -5524,7 +5524,7 @@
       <c r="Y47" s="1" t="n">
         <v>0.7</v>
       </c>
-      <c r="Z47" s="0" t="s">
+      <c r="Z47" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -5604,7 +5604,7 @@
       <c r="Y48" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="Z48" s="0" t="s">
+      <c r="Z48" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -5684,7 +5684,7 @@
       <c r="Y49" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="Z49" s="0" t="s">
+      <c r="Z49" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -5764,7 +5764,7 @@
       <c r="Y50" s="1" t="n">
         <v>1.2</v>
       </c>
-      <c r="Z50" s="0" t="s">
+      <c r="Z50" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -5844,7 +5844,7 @@
       <c r="Y51" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Z51" s="0" t="s">
+      <c r="Z51" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -5924,7 +5924,7 @@
       <c r="Y52" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="Z52" s="0" t="s">
+      <c r="Z52" s="1" t="s">
         <v>42</v>
       </c>
     </row>
@@ -6004,7 +6004,7 @@
       <c r="Y53" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Z53" s="0" t="s">
+      <c r="Z53" s="1" t="s">
         <v>315</v>
       </c>
     </row>
@@ -6084,7 +6084,7 @@
       <c r="Y54" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Z54" s="0" t="s">
+      <c r="Z54" s="1" t="s">
         <v>315</v>
       </c>
     </row>
@@ -6164,7 +6164,7 @@
       <c r="Y55" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="Z55" s="0" t="s">
+      <c r="Z55" s="1" t="s">
         <v>315</v>
       </c>
     </row>
@@ -6244,7 +6244,7 @@
       <c r="Y56" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="Z56" s="0" t="s">
+      <c r="Z56" s="1" t="s">
         <v>315</v>
       </c>
     </row>
@@ -6324,7 +6324,7 @@
       <c r="Y57" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="Z57" s="0" t="s">
+      <c r="Z57" s="1" t="s">
         <v>315</v>
       </c>
     </row>
@@ -6404,7 +6404,7 @@
       <c r="Y58" s="1" t="n">
         <v>0.9</v>
       </c>
-      <c r="Z58" s="0" t="s">
+      <c r="Z58" s="1" t="s">
         <v>315</v>
       </c>
     </row>
@@ -6484,7 +6484,7 @@
       <c r="Y59" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="Z59" s="0" t="s">
+      <c r="Z59" s="1" t="s">
         <v>315</v>
       </c>
     </row>
@@ -6564,7 +6564,7 @@
       <c r="Y60" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Z60" s="0" t="s">
+      <c r="Z60" s="1" t="s">
         <v>315</v>
       </c>
     </row>
@@ -6644,7 +6644,7 @@
       <c r="Y61" s="1" t="n">
         <v>1.8</v>
       </c>
-      <c r="Z61" s="0" t="s">
+      <c r="Z61" s="1" t="s">
         <v>315</v>
       </c>
     </row>
@@ -6724,7 +6724,7 @@
       <c r="Y62" s="1" t="n">
         <v>2.5</v>
       </c>
-      <c r="Z62" s="0" t="s">
+      <c r="Z62" s="1" t="s">
         <v>315</v>
       </c>
     </row>
@@ -6804,7 +6804,7 @@
       <c r="Y63" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="Z63" s="0" t="s">
+      <c r="Z63" s="1" t="s">
         <v>315</v>
       </c>
     </row>
@@ -6884,7 +6884,7 @@
       <c r="Y64" s="1" t="n">
         <v>90</v>
       </c>
-      <c r="Z64" s="0" t="s">
+      <c r="Z64" s="1" t="s">
         <v>315</v>
       </c>
     </row>
@@ -6964,7 +6964,7 @@
       <c r="Y65" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Z65" s="0" t="s">
+      <c r="Z65" s="1" t="s">
         <v>315</v>
       </c>
     </row>
@@ -7044,7 +7044,7 @@
       <c r="Y66" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Z66" s="0" t="s">
+      <c r="Z66" s="1" t="s">
         <v>315</v>
       </c>
     </row>
@@ -7124,7 +7124,7 @@
       <c r="Y67" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="Z67" s="0" t="s">
+      <c r="Z67" s="1" t="s">
         <v>315</v>
       </c>
     </row>
@@ -7204,7 +7204,7 @@
       <c r="Y68" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Z68" s="0" t="s">
+      <c r="Z68" s="1" t="s">
         <v>315</v>
       </c>
     </row>
@@ -7284,7 +7284,7 @@
       <c r="Y69" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="Z69" s="0" t="s">
+      <c r="Z69" s="1" t="s">
         <v>315</v>
       </c>
     </row>
@@ -7364,7 +7364,7 @@
       <c r="Y70" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="Z70" s="0" t="s">
+      <c r="Z70" s="1" t="s">
         <v>315</v>
       </c>
     </row>
@@ -7444,7 +7444,7 @@
       <c r="Y71" s="1" t="n">
         <v>1.5</v>
       </c>
-      <c r="Z71" s="0" t="s">
+      <c r="Z71" s="1" t="s">
         <v>315</v>
       </c>
     </row>
@@ -7524,7 +7524,7 @@
       <c r="Y72" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="Z72" s="0" t="s">
+      <c r="Z72" s="1" t="s">
         <v>315</v>
       </c>
     </row>
@@ -7604,7 +7604,7 @@
       <c r="Y73" s="1" t="n">
         <v>0.7</v>
       </c>
-      <c r="Z73" s="0" t="s">
+      <c r="Z73" s="1" t="s">
         <v>315</v>
       </c>
     </row>
@@ -7684,7 +7684,7 @@
       <c r="Y74" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="Z74" s="0" t="s">
+      <c r="Z74" s="1" t="s">
         <v>315</v>
       </c>
     </row>
@@ -7764,7 +7764,7 @@
       <c r="Y75" s="1" t="n">
         <v>1.2</v>
       </c>
-      <c r="Z75" s="0" t="s">
+      <c r="Z75" s="1" t="s">
         <v>315</v>
       </c>
     </row>
@@ -7844,7 +7844,7 @@
       <c r="Y76" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="Z76" s="0" t="s">
+      <c r="Z76" s="1" t="s">
         <v>315</v>
       </c>
     </row>
@@ -7909,7 +7909,7 @@
       <c r="Y77" s="1" t="n">
         <v>0.8</v>
       </c>
-      <c r="Z77" s="0" t="s">
+      <c r="Z77" s="1" t="s">
         <v>427</v>
       </c>
     </row>
@@ -7974,7 +7974,7 @@
       <c r="Y78" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="Z78" s="0" t="s">
+      <c r="Z78" s="1" t="s">
         <v>427</v>
       </c>
     </row>
@@ -8039,7 +8039,7 @@
       <c r="Y79" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="Z79" s="0" t="s">
+      <c r="Z79" s="1" t="s">
         <v>427</v>
       </c>
     </row>
@@ -8101,7 +8101,7 @@
       <c r="Y80" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="Z80" s="0" t="s">
+      <c r="Z80" s="1" t="s">
         <v>427</v>
       </c>
     </row>
@@ -8163,7 +8163,7 @@
       <c r="Y81" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="Z81" s="0" t="s">
+      <c r="Z81" s="1" t="s">
         <v>427</v>
       </c>
     </row>
@@ -8225,7 +8225,7 @@
       <c r="Y82" s="1" t="n">
         <v>0.5</v>
       </c>
-      <c r="Z82" s="0" t="s">
+      <c r="Z82" s="1" t="s">
         <v>427</v>
       </c>
     </row>
@@ -8287,7 +8287,7 @@
       <c r="Y83" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Z83" s="0" t="s">
+      <c r="Z83" s="1" t="s">
         <v>427</v>
       </c>
     </row>
@@ -8349,7 +8349,7 @@
       <c r="Y84" s="1" t="n">
         <v>0.6</v>
       </c>
-      <c r="Z84" s="0" t="s">
+      <c r="Z84" s="1" t="s">
         <v>460</v>
       </c>
     </row>
@@ -8411,7 +8411,7 @@
       <c r="Y85" s="1" t="n">
         <v>1.1</v>
       </c>
-      <c r="Z85" s="0" t="s">
+      <c r="Z85" s="1" t="s">
         <v>460</v>
       </c>
     </row>
@@ -8473,7 +8473,7 @@
       <c r="Y86" s="1" t="n">
         <v>1.6</v>
       </c>
-      <c r="Z86" s="0" t="s">
+      <c r="Z86" s="1" t="s">
         <v>460</v>
       </c>
     </row>
@@ -8535,7 +8535,7 @@
       <c r="Y87" s="1" t="n">
         <v>1.7</v>
       </c>
-      <c r="Z87" s="0" t="s">
+      <c r="Z87" s="1" t="s">
         <v>460</v>
       </c>
     </row>
@@ -8597,7 +8597,7 @@
       <c r="Y88" s="1" t="n">
         <v>0.7</v>
       </c>
-      <c r="Z88" s="0" t="s">
+      <c r="Z88" s="1" t="s">
         <v>460</v>
       </c>
     </row>
@@ -8659,7 +8659,7 @@
       <c r="Y89" s="1" t="n">
         <v>0.4</v>
       </c>
-      <c r="Z89" s="0" t="s">
+      <c r="Z89" s="1" t="s">
         <v>460</v>
       </c>
     </row>
@@ -8721,7 +8721,7 @@
       <c r="Y90" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Z90" s="0" t="s">
+      <c r="Z90" s="1" t="s">
         <v>460</v>
       </c>
     </row>
@@ -8783,7 +8783,7 @@
       <c r="Y91" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Z91" s="0" t="s">
+      <c r="Z91" s="1" t="s">
         <v>460</v>
       </c>
     </row>
@@ -8845,7 +8845,7 @@
       <c r="Y92" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Z92" s="0" t="s">
+      <c r="Z92" s="1" t="s">
         <v>460</v>
       </c>
     </row>
@@ -8907,7 +8907,7 @@
       <c r="Y93" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Z93" s="0" t="s">
+      <c r="Z93" s="1" t="s">
         <v>495</v>
       </c>
     </row>
@@ -8969,7 +8969,7 @@
       <c r="Y94" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Z94" s="0" t="s">
+      <c r="Z94" s="1" t="s">
         <v>504</v>
       </c>
     </row>
@@ -9031,7 +9031,7 @@
       <c r="Y95" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="Z95" s="0" t="s">
+      <c r="Z95" s="1" t="s">
         <v>513</v>
       </c>
     </row>

</xml_diff>